<commit_message>
Dodata opcija za postavljanje zeljene menze, izmenjen naziv naloga sa koga se salje
</commit_message>
<xml_diff>
--- a/exceldokument.xlsx
+++ b/exceldokument.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cloudconvert\server\files\tasks\ab5ad6bc-9421-43de-87b0-4f8fb75ec366\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\marko\python-menza\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9A3965D-F973-482D-93A1-BD2A83EABE52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="11520" windowHeight="7875"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="kapitalna  - korisnici" sheetId="5" r:id="rId1"/>
@@ -85,9 +84,6 @@
     <t>vreme</t>
   </si>
   <si>
-    <t>Trpezarija Kapitalna</t>
-  </si>
-  <si>
     <t>Vrsta kuvanog obroka</t>
   </si>
   <si>
@@ -107,6 +103,9 @@
   </si>
   <si>
     <t>**Rezervacija obroka se može izvršiti dan unapred do 08/00h ili PETKOM ZA NAREDNIH 7 DANA</t>
+  </si>
+  <si>
+    <t>Trpezarija</t>
   </si>
 </sst>
 </file>
@@ -434,23 +433,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -486,23 +468,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -682,7 +647,7 @@
   <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
@@ -733,7 +698,7 @@
     <row r="6" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="24" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -743,7 +708,7 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="36"/>
       <c r="D8" s="36"/>
@@ -752,7 +717,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>0</v>
@@ -761,7 +726,7 @@
         <v>3</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E10" s="30" t="s">
         <v>2</v>
@@ -1139,7 +1104,7 @@
     </row>
     <row r="47" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="40" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B47" s="41"/>
       <c r="C47" s="41"/>
@@ -1157,7 +1122,7 @@
     </row>
     <row r="49" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="37" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B49" s="38"/>
       <c r="C49" s="38"/>
@@ -1167,7 +1132,7 @@
     </row>
     <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="37" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B50" s="38"/>
       <c r="C50" s="38"/>
@@ -1282,7 +1247,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>1</v>

</xml_diff>